<commit_message>
Filtros de empenho na listagem principal.
</commit_message>
<xml_diff>
--- a/storage/ESTOQUE ATUALIZADO.xlsx
+++ b/storage/ESTOQUE ATUALIZADO.xlsx
@@ -50,7 +50,7 @@
     <t xml:space="preserve">COD. BARRAS</t>
   </si>
   <si>
-    <t xml:space="preserve">DESCRICAO</t>
+    <t xml:space="preserve">$r</t>
   </si>
   <si>
     <t xml:space="preserve">QUADRA</t>
@@ -403,10 +403,10 @@
   </sheetPr>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -416,7 +416,8 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.8380566801619"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9878542510121"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="71.663967611336"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="3" width="14.4615384615385"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="3" width="18.9595141700405"/>

</xml_diff>